<commit_message>
BJ: Update participant form.
</commit_message>
<xml_diff>
--- a/LF/TAS/Benin/Apr 2021/bj_lf_retas1_1_sites_202104.xlsx
+++ b/LF/TAS/Benin/Apr 2021/bj_lf_retas1_1_sites_202104.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\TAS\Benin\Apr 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FCD666-DDCF-4027-9847-5F700CAF8920}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D02156E-5C53-4F98-B899-E17846C0BC64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="197">
   <si>
     <t>form_title</t>
   </si>
@@ -317,18 +317,6 @@
     <t>c_cluster_name</t>
   </si>
   <si>
-    <t>Enter the school Name</t>
-  </si>
-  <si>
-    <t>Entrer le nom de l'école</t>
-  </si>
-  <si>
-    <t>c_cluster_id1</t>
-  </si>
-  <si>
-    <t>Entrer le code de l'école</t>
-  </si>
-  <si>
     <t>. &gt; 99 and .&lt; 1000</t>
   </si>
   <si>
@@ -344,46 +332,296 @@
     <t>Le code a trois chiffre associé à chaque école</t>
   </si>
   <si>
-    <t>c_cluster_id2</t>
-  </si>
-  <si>
-    <t>. = ${c_cluster_id1}</t>
-  </si>
-  <si>
-    <t>The code must be the same</t>
-  </si>
-  <si>
-    <t>Le code répété doit être le même</t>
-  </si>
-  <si>
-    <t>Enter the cluster ID</t>
-  </si>
-  <si>
-    <t>Repeat the cluster ID</t>
-  </si>
-  <si>
-    <t>Répéter le code de l'école</t>
-  </si>
-  <si>
-    <t>Covè</t>
-  </si>
-  <si>
-    <t>Ouinhi</t>
-  </si>
-  <si>
-    <t>Zagnanado</t>
-  </si>
-  <si>
-    <t>Za-Kpota</t>
-  </si>
-  <si>
-    <t>Cove</t>
-  </si>
-  <si>
-    <t>1. Benin - Re TAS1 FL Formulaire Site (Avril 2021) V2</t>
-  </si>
-  <si>
-    <t>bj_lf_retas1_1_sites_202104_v2</t>
+    <t>COVE</t>
+  </si>
+  <si>
+    <t>OUINHI</t>
+  </si>
+  <si>
+    <t>ZA-KPOTA</t>
+  </si>
+  <si>
+    <t>ZAGNANADO</t>
+  </si>
+  <si>
+    <t>EYRAM</t>
+  </si>
+  <si>
+    <t>LA REFERENCE (ADOGBE)</t>
+  </si>
+  <si>
+    <t>AHITO</t>
+  </si>
+  <si>
+    <t>GOUNLI/A</t>
+  </si>
+  <si>
+    <t>HOUNSO/C</t>
+  </si>
+  <si>
+    <t>LES GRANDES AMES</t>
+  </si>
+  <si>
+    <t>SOLI/A</t>
+  </si>
+  <si>
+    <t>ZOGBA/A</t>
+  </si>
+  <si>
+    <t>ADJOKAN / C</t>
+  </si>
+  <si>
+    <t>ADJOKAN HOUAWO / B</t>
+  </si>
+  <si>
+    <t>SOWEKPA</t>
+  </si>
+  <si>
+    <t>FOLLY</t>
+  </si>
+  <si>
+    <t>KOGUEDE / B</t>
+  </si>
+  <si>
+    <t>AFFOSSOWAGBA</t>
+  </si>
+  <si>
+    <t>KPAKPAME / B</t>
+  </si>
+  <si>
+    <t>ZA DRAME / A</t>
+  </si>
+  <si>
+    <t>KPOZOUN / C</t>
+  </si>
+  <si>
+    <t>KPOZOUN / A</t>
+  </si>
+  <si>
+    <t>Adjido A</t>
+  </si>
+  <si>
+    <t>LE SUCCES D'ADJIDO</t>
+  </si>
+  <si>
+    <t>SAINTE THERESE DE L'ENFANT JESUS</t>
+  </si>
+  <si>
+    <t>ZA KPOTA / A</t>
+  </si>
+  <si>
+    <t>ZA KPOTA CENTRE / B</t>
+  </si>
+  <si>
+    <t>LA PERSEVERANCE</t>
+  </si>
+  <si>
+    <t>ZA AGONDOKPOE / A</t>
+  </si>
+  <si>
+    <t>ZA TANTA / B</t>
+  </si>
+  <si>
+    <t>LA REFERENCE (ZEKO)</t>
+  </si>
+  <si>
+    <t>TANGBEKPA</t>
+  </si>
+  <si>
+    <t>ZEKO / B</t>
+  </si>
+  <si>
+    <t>ZEKO QUARTIER</t>
+  </si>
+  <si>
+    <t>EPP Dasso B</t>
+  </si>
+  <si>
+    <t>AHICON</t>
+  </si>
+  <si>
+    <t>HOLLI</t>
+  </si>
+  <si>
+    <t>LE PROGRES</t>
+  </si>
+  <si>
+    <t>MAFOUNGBON</t>
+  </si>
+  <si>
+    <t>MONZOUNGOUDO</t>
+  </si>
+  <si>
+    <t>ODJA ODAN</t>
+  </si>
+  <si>
+    <t>OUOKON AHLAN</t>
+  </si>
+  <si>
+    <t>ADAGBODJI</t>
+  </si>
+  <si>
+    <t>AIZE / B</t>
+  </si>
+  <si>
+    <t>DOLIVI</t>
+  </si>
+  <si>
+    <t>OZOKPODI</t>
+  </si>
+  <si>
+    <t>TEZOUNME</t>
+  </si>
+  <si>
+    <t>EPP Aissin 
+Dangbehoue</t>
+  </si>
+  <si>
+    <t>AGBLADOHO</t>
+  </si>
+  <si>
+    <t>AKOHAGON</t>
+  </si>
+  <si>
+    <t>BOCONONGON</t>
+  </si>
+  <si>
+    <t>BODEDJI</t>
+  </si>
+  <si>
+    <t>HELOUTEDJI</t>
+  </si>
+  <si>
+    <t>MASSAGBO</t>
+  </si>
+  <si>
+    <t>ZOBLAGADA</t>
+  </si>
+  <si>
+    <t>DON / A</t>
+  </si>
+  <si>
+    <t>DON / B</t>
+  </si>
+  <si>
+    <t>GOBLIDJI</t>
+  </si>
+  <si>
+    <t>DOVI DOVE / A</t>
+  </si>
+  <si>
+    <t>AZAKPA</t>
+  </si>
+  <si>
+    <t>IGBO OLA</t>
+  </si>
+  <si>
+    <t>WOMETO GLONZOUME</t>
+  </si>
+  <si>
+    <t>LA JEUNESSE AMBITION</t>
+  </si>
+  <si>
+    <t>ZAGNANADO CENTRE</t>
+  </si>
+  <si>
+    <t>COVE/C</t>
+  </si>
+  <si>
+    <t>DOVI COGBE</t>
+  </si>
+  <si>
+    <t>TOKPLEGBE/B</t>
+  </si>
+  <si>
+    <t>CATHOLIQUE SAINT AUGUSTIN</t>
+  </si>
+  <si>
+    <t>ZOGBA/B</t>
+  </si>
+  <si>
+    <t>HOUNGOME</t>
+  </si>
+  <si>
+    <t>DRAME TANDJI</t>
+  </si>
+  <si>
+    <t>DJOYITIN / A</t>
+  </si>
+  <si>
+    <t>KPOZOUN / B</t>
+  </si>
+  <si>
+    <t>ALLOHOUN OUNKANME / B</t>
+  </si>
+  <si>
+    <t>GNANLI ZOUNGUE / C</t>
+  </si>
+  <si>
+    <t>MIDJANNAGAN</t>
+  </si>
+  <si>
+    <t>WOKPA</t>
+  </si>
+  <si>
+    <t>ADADJAGON</t>
+  </si>
+  <si>
+    <t>DOVI ZOUNOU</t>
+  </si>
+  <si>
+    <t>AGONGBODJI / B</t>
+  </si>
+  <si>
+    <t>AGONVE</t>
+  </si>
+  <si>
+    <t>AHLAN</t>
+  </si>
+  <si>
+    <t>KPOTO</t>
+  </si>
+  <si>
+    <t>DOGA ZOUNGOUDO / B</t>
+  </si>
+  <si>
+    <t>site_list</t>
+  </si>
+  <si>
+    <t>site_ids</t>
+  </si>
+  <si>
+    <t>select_one site_list</t>
+  </si>
+  <si>
+    <t>select_one site_ids</t>
+  </si>
+  <si>
+    <t>c_cluster_id</t>
+  </si>
+  <si>
+    <t>bj_lf_retas1_1_sites_202104_v3</t>
+  </si>
+  <si>
+    <t>Sélectionner le nom de l'école</t>
+  </si>
+  <si>
+    <t>Sélectionner le code de l'école</t>
+  </si>
+  <si>
+    <t>Select the school Name</t>
+  </si>
+  <si>
+    <t>Select the cluster ID</t>
+  </si>
+  <si>
+    <t>1. Benin - Re TAS1 FL Formulaire Site (Avril 2021) V3</t>
+  </si>
+  <si>
+    <t>commune_list = ${c_commune}</t>
+  </si>
+  <si>
+    <t>site_list = ${c_cluster_name}</t>
   </si>
 </sst>
 </file>
@@ -907,13 +1145,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1084,17 +1322,17 @@
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="11" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="14"/>
@@ -1108,36 +1346,38 @@
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>40</v>
+        <v>187</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
@@ -1146,55 +1386,51 @@
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
-      <c r="P6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>109</v>
+      <c r="P6" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="11" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="8"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="9"/>
@@ -1210,105 +1446,113 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" s="14"/>
       <c r="M10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
     </row>
     <row r="11" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+        <v>24</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="K11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L11" s="14"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="21" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="8"/>
@@ -1316,10 +1560,10 @@
         <v>57</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>88</v>
@@ -1332,31 +1576,29 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="20"/>
+        <v>51</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>38</v>
+      </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
       <c r="K13" s="1" t="s">
         <v>88</v>
       </c>
@@ -1369,73 +1611,63 @@
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>27</v>
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>29</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D14" s="20"/>
       <c r="E14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+        <v>86</v>
+      </c>
+      <c r="F14" s="21"/>
       <c r="K14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="M14" s="33"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="21" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="F15" s="21"/>
-      <c r="K15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="33"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D16" s="20"/>
-      <c r="E16" s="21" t="s">
-        <v>39</v>
-      </c>
+      <c r="E16" s="21"/>
       <c r="F16" s="21"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1450,10 +1682,10 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>33</v>
@@ -1472,30 +1704,6 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1504,11 +1712,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1517,10 +1725,10 @@
     <col min="2" max="2" width="39.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
@@ -1536,152 +1744,3052 @@
       <c r="E1" s="26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E2" s="35"/>
     </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E3" s="35"/>
     </row>
-    <row r="4" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
       <c r="B4" s="34"/>
       <c r="C4" s="31"/>
       <c r="D4" s="32"/>
       <c r="E4" s="35"/>
     </row>
-    <row r="5" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27"/>
       <c r="B9" s="34"/>
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
-      <c r="E9" s="35"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="34"/>
+      <c r="F12" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="34"/>
+      <c r="F14" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="34"/>
+      <c r="F15" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="34"/>
+      <c r="F17" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="34"/>
+      <c r="F18" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="34"/>
+      <c r="F21" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="F29" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="F30" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="34"/>
+      <c r="F31" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="F32" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="34"/>
+      <c r="F34" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="34"/>
+      <c r="F35" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="34"/>
+      <c r="F39" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="34"/>
+      <c r="F40" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="34"/>
+      <c r="F42" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="34"/>
+      <c r="F43" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="34"/>
+      <c r="F44" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="34"/>
+      <c r="F45" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="34"/>
+      <c r="F46" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="34"/>
+      <c r="F48" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="34"/>
+      <c r="F49" s="36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50" s="34"/>
+      <c r="F50" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="34"/>
+      <c r="F51" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E52" s="34"/>
+      <c r="F52" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="34"/>
+      <c r="F53" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" s="34"/>
+      <c r="F54" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56" s="34"/>
+      <c r="F56" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="E57" s="34"/>
+      <c r="F57" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E58" s="34"/>
+      <c r="F58" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="D59" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="E59" s="34"/>
+      <c r="F59" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" s="34"/>
+      <c r="F60" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="E61" s="34"/>
+      <c r="F61" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E62" s="34"/>
+      <c r="F62" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="34"/>
+      <c r="F63" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" s="34"/>
+      <c r="F64" s="36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="E65" s="34"/>
+      <c r="F65" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="E66" s="34"/>
+      <c r="F66" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="E67" s="34"/>
+      <c r="F67" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C68" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="E68" s="34"/>
+      <c r="F68" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" s="34"/>
+      <c r="F69" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="E70" s="34"/>
+      <c r="F70" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="34"/>
+      <c r="F71" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B72" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="34"/>
+      <c r="F72" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D73" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E73" s="34"/>
+      <c r="F73" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D74" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="E74" s="34"/>
+      <c r="F74" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B75" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C75" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="E75" s="34"/>
+      <c r="F75" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C76" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="E76" s="34"/>
+      <c r="F76" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="D77" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" s="34"/>
+      <c r="F77" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="C78" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="D78" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="E78" s="34"/>
+      <c r="F78" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D79" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="E79" s="34"/>
+      <c r="F79" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B80" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D80" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E80" s="34"/>
+      <c r="F80" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D81" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E81" s="34"/>
+      <c r="F81" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="E82" s="34"/>
+      <c r="F82" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="D83" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E83" s="34"/>
+      <c r="F83" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B84" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="D84" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="E84" s="34"/>
+      <c r="F84" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B85" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C85" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E85" s="34"/>
+      <c r="F85" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="E86" s="34"/>
+      <c r="F86" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="D87" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E87" s="34"/>
+      <c r="F87" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="D88" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="E88" s="34"/>
+      <c r="F88" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B89" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C89" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D89" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="E89" s="34"/>
+      <c r="F89" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="27"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="31"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="34"/>
+    </row>
+    <row r="91" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B91" s="34">
+        <v>100</v>
+      </c>
+      <c r="C91" s="31">
+        <v>100</v>
+      </c>
+      <c r="D91" s="32">
+        <v>100</v>
+      </c>
+      <c r="E91" s="34"/>
+      <c r="G91" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" s="34">
+        <v>101</v>
+      </c>
+      <c r="C92" s="31">
+        <v>101</v>
+      </c>
+      <c r="D92" s="32">
+        <v>101</v>
+      </c>
+      <c r="E92" s="34"/>
+      <c r="G92" s="36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B93" s="34">
+        <v>102</v>
+      </c>
+      <c r="C93" s="31">
+        <v>102</v>
+      </c>
+      <c r="D93" s="32">
+        <v>102</v>
+      </c>
+      <c r="E93" s="34"/>
+      <c r="G93" s="36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="34">
+        <v>103</v>
+      </c>
+      <c r="C94" s="31">
+        <v>103</v>
+      </c>
+      <c r="D94" s="32">
+        <v>103</v>
+      </c>
+      <c r="E94" s="34"/>
+      <c r="G94" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B95" s="34">
+        <v>104</v>
+      </c>
+      <c r="C95" s="31">
+        <v>104</v>
+      </c>
+      <c r="D95" s="32">
+        <v>104</v>
+      </c>
+      <c r="E95" s="34"/>
+      <c r="G95" s="36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B96" s="34">
+        <v>105</v>
+      </c>
+      <c r="C96" s="31">
+        <v>105</v>
+      </c>
+      <c r="D96" s="32">
+        <v>105</v>
+      </c>
+      <c r="E96" s="34"/>
+      <c r="G96" s="36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" s="34">
+        <v>106</v>
+      </c>
+      <c r="C97" s="31">
+        <v>106</v>
+      </c>
+      <c r="D97" s="32">
+        <v>106</v>
+      </c>
+      <c r="E97" s="34"/>
+      <c r="G97" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B98" s="34">
+        <v>107</v>
+      </c>
+      <c r="C98" s="31">
+        <v>107</v>
+      </c>
+      <c r="D98" s="32">
+        <v>107</v>
+      </c>
+      <c r="E98" s="34"/>
+      <c r="G98" s="36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B99" s="34">
+        <v>108</v>
+      </c>
+      <c r="C99" s="31">
+        <v>108</v>
+      </c>
+      <c r="D99" s="32">
+        <v>108</v>
+      </c>
+      <c r="E99" s="34"/>
+      <c r="G99" s="36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B100" s="34">
+        <v>109</v>
+      </c>
+      <c r="C100" s="31">
+        <v>109</v>
+      </c>
+      <c r="D100" s="32">
+        <v>109</v>
+      </c>
+      <c r="E100" s="34"/>
+      <c r="G100" s="36" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="34">
+        <v>110</v>
+      </c>
+      <c r="C101" s="31">
+        <v>110</v>
+      </c>
+      <c r="D101" s="32">
+        <v>110</v>
+      </c>
+      <c r="E101" s="34"/>
+      <c r="G101" s="36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="34">
+        <v>111</v>
+      </c>
+      <c r="C102" s="31">
+        <v>111</v>
+      </c>
+      <c r="D102" s="32">
+        <v>111</v>
+      </c>
+      <c r="E102" s="34"/>
+      <c r="G102" s="36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B103" s="34">
+        <v>112</v>
+      </c>
+      <c r="C103" s="31">
+        <v>112</v>
+      </c>
+      <c r="D103" s="32">
+        <v>112</v>
+      </c>
+      <c r="E103" s="34"/>
+      <c r="G103" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B104" s="34">
+        <v>113</v>
+      </c>
+      <c r="C104" s="31">
+        <v>113</v>
+      </c>
+      <c r="D104" s="32">
+        <v>113</v>
+      </c>
+      <c r="E104" s="34"/>
+      <c r="G104" s="36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B105" s="34">
+        <v>114</v>
+      </c>
+      <c r="C105" s="31">
+        <v>114</v>
+      </c>
+      <c r="D105" s="32">
+        <v>114</v>
+      </c>
+      <c r="E105" s="34"/>
+      <c r="G105" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" s="34">
+        <v>115</v>
+      </c>
+      <c r="C106" s="31">
+        <v>115</v>
+      </c>
+      <c r="D106" s="32">
+        <v>115</v>
+      </c>
+      <c r="E106" s="34"/>
+      <c r="G106" s="36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B107" s="34">
+        <v>116</v>
+      </c>
+      <c r="C107" s="31">
+        <v>116</v>
+      </c>
+      <c r="D107" s="32">
+        <v>116</v>
+      </c>
+      <c r="E107" s="34"/>
+      <c r="G107" s="36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B108" s="34">
+        <v>117</v>
+      </c>
+      <c r="C108" s="31">
+        <v>117</v>
+      </c>
+      <c r="D108" s="32">
+        <v>117</v>
+      </c>
+      <c r="E108" s="34"/>
+      <c r="G108" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B109" s="34">
+        <v>118</v>
+      </c>
+      <c r="C109" s="31">
+        <v>118</v>
+      </c>
+      <c r="D109" s="32">
+        <v>118</v>
+      </c>
+      <c r="E109" s="34"/>
+      <c r="G109" s="36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B110" s="34">
+        <v>119</v>
+      </c>
+      <c r="C110" s="31">
+        <v>119</v>
+      </c>
+      <c r="D110" s="32">
+        <v>119</v>
+      </c>
+      <c r="E110" s="34"/>
+      <c r="G110" s="36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" s="34">
+        <v>120</v>
+      </c>
+      <c r="C111" s="31">
+        <v>120</v>
+      </c>
+      <c r="D111" s="32">
+        <v>120</v>
+      </c>
+      <c r="E111" s="34"/>
+      <c r="G111" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B112" s="34">
+        <v>121</v>
+      </c>
+      <c r="C112" s="31">
+        <v>121</v>
+      </c>
+      <c r="D112" s="32">
+        <v>121</v>
+      </c>
+      <c r="E112" s="34"/>
+      <c r="G112" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B113" s="34">
+        <v>122</v>
+      </c>
+      <c r="C113" s="31">
+        <v>122</v>
+      </c>
+      <c r="D113" s="32">
+        <v>122</v>
+      </c>
+      <c r="E113" s="34"/>
+      <c r="G113" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B114" s="34">
+        <v>123</v>
+      </c>
+      <c r="C114" s="31">
+        <v>123</v>
+      </c>
+      <c r="D114" s="32">
+        <v>123</v>
+      </c>
+      <c r="E114" s="34"/>
+      <c r="G114" s="36" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B115" s="34">
+        <v>124</v>
+      </c>
+      <c r="C115" s="31">
+        <v>124</v>
+      </c>
+      <c r="D115" s="32">
+        <v>124</v>
+      </c>
+      <c r="E115" s="34"/>
+      <c r="G115" s="36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B116" s="34">
+        <v>125</v>
+      </c>
+      <c r="C116" s="31">
+        <v>125</v>
+      </c>
+      <c r="D116" s="32">
+        <v>125</v>
+      </c>
+      <c r="E116" s="34"/>
+      <c r="G116" s="36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="34">
+        <v>126</v>
+      </c>
+      <c r="C117" s="31">
+        <v>126</v>
+      </c>
+      <c r="D117" s="32">
+        <v>126</v>
+      </c>
+      <c r="E117" s="34"/>
+      <c r="G117" s="36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B118" s="34">
+        <v>127</v>
+      </c>
+      <c r="C118" s="31">
+        <v>127</v>
+      </c>
+      <c r="D118" s="32">
+        <v>127</v>
+      </c>
+      <c r="E118" s="34"/>
+      <c r="G118" s="36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B119" s="34">
+        <v>128</v>
+      </c>
+      <c r="C119" s="31">
+        <v>128</v>
+      </c>
+      <c r="D119" s="32">
+        <v>128</v>
+      </c>
+      <c r="E119" s="34"/>
+      <c r="G119" s="36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B120" s="34">
+        <v>129</v>
+      </c>
+      <c r="C120" s="31">
+        <v>129</v>
+      </c>
+      <c r="D120" s="32">
+        <v>129</v>
+      </c>
+      <c r="E120" s="34"/>
+      <c r="G120" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B121" s="34">
+        <v>130</v>
+      </c>
+      <c r="C121" s="31">
+        <v>130</v>
+      </c>
+      <c r="D121" s="32">
+        <v>130</v>
+      </c>
+      <c r="E121" s="34"/>
+      <c r="G121" s="36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B122" s="34">
+        <v>131</v>
+      </c>
+      <c r="C122" s="31">
+        <v>131</v>
+      </c>
+      <c r="D122" s="32">
+        <v>131</v>
+      </c>
+      <c r="E122" s="34"/>
+      <c r="G122" s="36" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B123" s="34">
+        <v>132</v>
+      </c>
+      <c r="C123" s="31">
+        <v>132</v>
+      </c>
+      <c r="D123" s="32">
+        <v>132</v>
+      </c>
+      <c r="E123" s="34"/>
+      <c r="G123" s="36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B124" s="34">
+        <v>133</v>
+      </c>
+      <c r="C124" s="31">
+        <v>133</v>
+      </c>
+      <c r="D124" s="32">
+        <v>133</v>
+      </c>
+      <c r="E124" s="34"/>
+      <c r="G124" s="36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B125" s="34">
+        <v>134</v>
+      </c>
+      <c r="C125" s="31">
+        <v>134</v>
+      </c>
+      <c r="D125" s="32">
+        <v>134</v>
+      </c>
+      <c r="E125" s="34"/>
+      <c r="G125" s="36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B126" s="34">
+        <v>135</v>
+      </c>
+      <c r="C126" s="31">
+        <v>135</v>
+      </c>
+      <c r="D126" s="32">
+        <v>135</v>
+      </c>
+      <c r="E126" s="34"/>
+      <c r="G126" s="36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B127" s="34">
+        <v>136</v>
+      </c>
+      <c r="C127" s="31">
+        <v>136</v>
+      </c>
+      <c r="D127" s="32">
+        <v>136</v>
+      </c>
+      <c r="E127" s="34"/>
+      <c r="G127" s="36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B128" s="34">
+        <v>137</v>
+      </c>
+      <c r="C128" s="31">
+        <v>137</v>
+      </c>
+      <c r="D128" s="32">
+        <v>137</v>
+      </c>
+      <c r="E128" s="34"/>
+      <c r="G128" s="36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B129" s="34">
+        <v>138</v>
+      </c>
+      <c r="C129" s="31">
+        <v>138</v>
+      </c>
+      <c r="D129" s="32">
+        <v>138</v>
+      </c>
+      <c r="E129" s="34"/>
+      <c r="G129" s="36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B130" s="34">
+        <v>139</v>
+      </c>
+      <c r="C130" s="31">
+        <v>139</v>
+      </c>
+      <c r="D130" s="32">
+        <v>139</v>
+      </c>
+      <c r="E130" s="34"/>
+      <c r="G130" s="36" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B131" s="34">
+        <v>140</v>
+      </c>
+      <c r="C131" s="31">
+        <v>140</v>
+      </c>
+      <c r="D131" s="32">
+        <v>140</v>
+      </c>
+      <c r="E131" s="34"/>
+      <c r="G131" s="36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B132" s="34">
+        <v>141</v>
+      </c>
+      <c r="C132" s="31">
+        <v>141</v>
+      </c>
+      <c r="D132" s="32">
+        <v>141</v>
+      </c>
+      <c r="E132" s="34"/>
+      <c r="G132" s="36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B133" s="34">
+        <v>142</v>
+      </c>
+      <c r="C133" s="31">
+        <v>142</v>
+      </c>
+      <c r="D133" s="32">
+        <v>142</v>
+      </c>
+      <c r="E133" s="34"/>
+      <c r="G133" s="36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B134" s="34">
+        <v>143</v>
+      </c>
+      <c r="C134" s="31">
+        <v>143</v>
+      </c>
+      <c r="D134" s="32">
+        <v>143</v>
+      </c>
+      <c r="E134" s="34"/>
+      <c r="G134" s="36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B135" s="34">
+        <v>144</v>
+      </c>
+      <c r="C135" s="31">
+        <v>144</v>
+      </c>
+      <c r="D135" s="32">
+        <v>144</v>
+      </c>
+      <c r="E135" s="34"/>
+      <c r="G135" s="36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B136" s="34">
+        <v>145</v>
+      </c>
+      <c r="C136" s="31">
+        <v>145</v>
+      </c>
+      <c r="D136" s="32">
+        <v>145</v>
+      </c>
+      <c r="E136" s="34"/>
+      <c r="G136" s="36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B137" s="34">
+        <v>146</v>
+      </c>
+      <c r="C137" s="31">
+        <v>146</v>
+      </c>
+      <c r="D137" s="32">
+        <v>146</v>
+      </c>
+      <c r="E137" s="34"/>
+      <c r="G137" s="36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B138" s="34">
+        <v>147</v>
+      </c>
+      <c r="C138" s="31">
+        <v>147</v>
+      </c>
+      <c r="D138" s="32">
+        <v>147</v>
+      </c>
+      <c r="E138" s="34"/>
+      <c r="G138" s="36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B139" s="34">
+        <v>148</v>
+      </c>
+      <c r="C139" s="31">
+        <v>148</v>
+      </c>
+      <c r="D139" s="32">
+        <v>148</v>
+      </c>
+      <c r="E139" s="34"/>
+      <c r="G139" s="36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B140" s="34">
+        <v>149</v>
+      </c>
+      <c r="C140" s="31">
+        <v>149</v>
+      </c>
+      <c r="D140" s="32">
+        <v>149</v>
+      </c>
+      <c r="E140" s="34"/>
+      <c r="G140" s="36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B141" s="34">
+        <v>150</v>
+      </c>
+      <c r="C141" s="31">
+        <v>150</v>
+      </c>
+      <c r="D141" s="32">
+        <v>150</v>
+      </c>
+      <c r="E141" s="34"/>
+      <c r="G141" s="36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B142" s="34">
+        <v>151</v>
+      </c>
+      <c r="C142" s="31">
+        <v>151</v>
+      </c>
+      <c r="D142" s="32">
+        <v>151</v>
+      </c>
+      <c r="E142" s="34"/>
+      <c r="G142" s="36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B143" s="34">
+        <v>152</v>
+      </c>
+      <c r="C143" s="31">
+        <v>152</v>
+      </c>
+      <c r="D143" s="32">
+        <v>152</v>
+      </c>
+      <c r="E143" s="34"/>
+      <c r="G143" s="36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B144" s="34">
+        <v>153</v>
+      </c>
+      <c r="C144" s="31">
+        <v>153</v>
+      </c>
+      <c r="D144" s="32">
+        <v>153</v>
+      </c>
+      <c r="E144" s="34"/>
+      <c r="G144" s="36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B145" s="34">
+        <v>154</v>
+      </c>
+      <c r="C145" s="31">
+        <v>154</v>
+      </c>
+      <c r="D145" s="32">
+        <v>154</v>
+      </c>
+      <c r="E145" s="34"/>
+      <c r="G145" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B146" s="34">
+        <v>155</v>
+      </c>
+      <c r="C146" s="31">
+        <v>155</v>
+      </c>
+      <c r="D146" s="32">
+        <v>155</v>
+      </c>
+      <c r="E146" s="34"/>
+      <c r="G146" s="36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B147" s="34">
+        <v>156</v>
+      </c>
+      <c r="C147" s="31">
+        <v>156</v>
+      </c>
+      <c r="D147" s="32">
+        <v>156</v>
+      </c>
+      <c r="E147" s="34"/>
+      <c r="G147" s="36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B148" s="34">
+        <v>157</v>
+      </c>
+      <c r="C148" s="31">
+        <v>157</v>
+      </c>
+      <c r="D148" s="32">
+        <v>157</v>
+      </c>
+      <c r="E148" s="34"/>
+      <c r="G148" s="36" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B149" s="34">
+        <v>158</v>
+      </c>
+      <c r="C149" s="31">
+        <v>158</v>
+      </c>
+      <c r="D149" s="32">
+        <v>158</v>
+      </c>
+      <c r="E149" s="34"/>
+      <c r="G149" s="36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B150" s="34">
+        <v>159</v>
+      </c>
+      <c r="C150" s="31">
+        <v>159</v>
+      </c>
+      <c r="D150" s="32">
+        <v>159</v>
+      </c>
+      <c r="E150" s="34"/>
+      <c r="G150" s="36" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B151" s="34">
+        <v>160</v>
+      </c>
+      <c r="C151" s="31">
+        <v>160</v>
+      </c>
+      <c r="D151" s="32">
+        <v>160</v>
+      </c>
+      <c r="E151" s="34"/>
+      <c r="G151" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B152" s="34">
+        <v>161</v>
+      </c>
+      <c r="C152" s="31">
+        <v>161</v>
+      </c>
+      <c r="D152" s="32">
+        <v>161</v>
+      </c>
+      <c r="E152" s="34"/>
+      <c r="G152" s="36" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B153" s="34">
+        <v>162</v>
+      </c>
+      <c r="C153" s="31">
+        <v>162</v>
+      </c>
+      <c r="D153" s="32">
+        <v>162</v>
+      </c>
+      <c r="E153" s="34"/>
+      <c r="G153" s="36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B154" s="34">
+        <v>163</v>
+      </c>
+      <c r="C154" s="31">
+        <v>163</v>
+      </c>
+      <c r="D154" s="32">
+        <v>163</v>
+      </c>
+      <c r="E154" s="34"/>
+      <c r="G154" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B155" s="34">
+        <v>164</v>
+      </c>
+      <c r="C155" s="31">
+        <v>164</v>
+      </c>
+      <c r="D155" s="32">
+        <v>164</v>
+      </c>
+      <c r="E155" s="34"/>
+      <c r="G155" s="36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B156" s="34">
+        <v>165</v>
+      </c>
+      <c r="C156" s="31">
+        <v>165</v>
+      </c>
+      <c r="D156" s="32">
+        <v>165</v>
+      </c>
+      <c r="E156" s="34"/>
+      <c r="G156" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B157" s="34">
+        <v>166</v>
+      </c>
+      <c r="C157" s="31">
+        <v>166</v>
+      </c>
+      <c r="D157" s="32">
+        <v>166</v>
+      </c>
+      <c r="E157" s="34"/>
+      <c r="G157" s="36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B158" s="34">
+        <v>167</v>
+      </c>
+      <c r="C158" s="31">
+        <v>167</v>
+      </c>
+      <c r="D158" s="32">
+        <v>167</v>
+      </c>
+      <c r="E158" s="34"/>
+      <c r="G158" s="36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B159" s="34">
+        <v>168</v>
+      </c>
+      <c r="C159" s="31">
+        <v>168</v>
+      </c>
+      <c r="D159" s="32">
+        <v>168</v>
+      </c>
+      <c r="E159" s="34"/>
+      <c r="G159" s="36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B160" s="34">
+        <v>169</v>
+      </c>
+      <c r="C160" s="31">
+        <v>169</v>
+      </c>
+      <c r="D160" s="32">
+        <v>169</v>
+      </c>
+      <c r="E160" s="34"/>
+      <c r="G160" s="36" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B161" s="34">
+        <v>170</v>
+      </c>
+      <c r="C161" s="31">
+        <v>170</v>
+      </c>
+      <c r="D161" s="32">
+        <v>170</v>
+      </c>
+      <c r="E161" s="34"/>
+      <c r="G161" s="36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B162" s="34">
+        <v>171</v>
+      </c>
+      <c r="C162" s="31">
+        <v>171</v>
+      </c>
+      <c r="D162" s="32">
+        <v>171</v>
+      </c>
+      <c r="E162" s="34"/>
+      <c r="G162" s="36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B163" s="34">
+        <v>172</v>
+      </c>
+      <c r="C163" s="31">
+        <v>172</v>
+      </c>
+      <c r="D163" s="32">
+        <v>172</v>
+      </c>
+      <c r="E163" s="34"/>
+      <c r="G163" s="36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B164" s="34">
+        <v>173</v>
+      </c>
+      <c r="C164" s="31">
+        <v>173</v>
+      </c>
+      <c r="D164" s="32">
+        <v>173</v>
+      </c>
+      <c r="E164" s="34"/>
+      <c r="G164" s="36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B165" s="34">
+        <v>174</v>
+      </c>
+      <c r="C165" s="31">
+        <v>174</v>
+      </c>
+      <c r="D165" s="32">
+        <v>174</v>
+      </c>
+      <c r="E165" s="34"/>
+      <c r="G165" s="36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B166" s="34">
+        <v>175</v>
+      </c>
+      <c r="C166" s="31">
+        <v>175</v>
+      </c>
+      <c r="D166" s="32">
+        <v>175</v>
+      </c>
+      <c r="E166" s="34"/>
+      <c r="G166" s="36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B167" s="34">
+        <v>176</v>
+      </c>
+      <c r="C167" s="31">
+        <v>176</v>
+      </c>
+      <c r="D167" s="32">
+        <v>176</v>
+      </c>
+      <c r="E167" s="34"/>
+      <c r="G167" s="36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B168" s="34">
+        <v>177</v>
+      </c>
+      <c r="C168" s="31">
+        <v>177</v>
+      </c>
+      <c r="D168" s="32">
+        <v>177</v>
+      </c>
+      <c r="E168" s="34"/>
+      <c r="G168" s="36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B169" s="34">
+        <v>178</v>
+      </c>
+      <c r="C169" s="31">
+        <v>178</v>
+      </c>
+      <c r="D169" s="32">
+        <v>178</v>
+      </c>
+      <c r="E169" s="34"/>
+      <c r="G169" s="36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B170" s="34">
+        <v>179</v>
+      </c>
+      <c r="C170" s="31">
+        <v>179</v>
+      </c>
+      <c r="D170" s="32">
+        <v>179</v>
+      </c>
+      <c r="E170" s="34"/>
+      <c r="G170" s="36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="27"/>
+      <c r="B171" s="34"/>
+      <c r="C171" s="31"/>
+      <c r="D171" s="32"/>
+      <c r="E171" s="34"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B172" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C172" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D172" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="E172" s="27"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B173" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C173" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D173" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E173" s="27"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:C60">
-    <sortCondition ref="B15:B60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A177:C222">
+    <sortCondition ref="B177:B222"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1691,14 +4799,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.125" customWidth="1"/>
-    <col min="2" max="2" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1718,13 +4826,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>189</v>
       </c>
       <c r="C2">
-        <v>20210412</v>
+        <v>202104522</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>

</xml_diff>